<commit_message>
cap nhat 6 thang 9 nam 2023
</commit_message>
<xml_diff>
--- a/Luận văn GITHUB.xlsx
+++ b/Luận văn GITHUB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LVTN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7F90B5-7FB2-43AF-BB83-DA75A1934284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088C55A8-2409-4E15-B277-F382F0BB5B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{F613D93C-81B0-455C-B6DD-EA6E57B6EA76}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="205">
   <si>
     <t>STT</t>
   </si>
@@ -636,6 +636,12 @@
   </si>
   <si>
     <t>Đã cài đặt, chưa kiểm tra</t>
+  </si>
+  <si>
+    <t>Hình Minh Họa</t>
+  </si>
+  <si>
+    <t>z</t>
   </si>
 </sst>
 </file>
@@ -2937,10 +2943,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76849178-7D8E-40D5-805E-F1C496D5B8E9}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:G7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3006,11 +3012,11 @@
         <v>202</v>
       </c>
       <c r="H2" s="11">
-        <f>COUNTIF(D2:D39,"x")</f>
-        <v>18</v>
+        <f>COUNTIF(D2:D40,"x")</f>
+        <v>22</v>
       </c>
       <c r="I2" s="11">
-        <f>COUNTIF(E2:E39,"x")</f>
+        <f>COUNTIF(E2:E40,"x")</f>
         <v>0</v>
       </c>
     </row>
@@ -3038,36 +3044,44 @@
       <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+      <c r="A4" s="14">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="G4" s="12"/>
+      <c r="G4" s="15" t="s">
+        <v>202</v>
+      </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="A5" s="14">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12" t="s">
+      <c r="C5" s="16"/>
+      <c r="D5" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="G5" s="12"/>
+      <c r="G5" s="15" t="s">
+        <v>202</v>
+      </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
@@ -3118,7 +3132,7 @@
       <c r="I7" s="12"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
+      <c r="A8" s="14">
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -3135,7 +3149,7 @@
       <c r="I8" s="12"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
+      <c r="A9" s="14">
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -3166,7 +3180,7 @@
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15" t="s">
-        <v>24</v>
+        <v>204</v>
       </c>
       <c r="G10" s="15" t="s">
         <v>202</v>
@@ -3248,7 +3262,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>191</v>
@@ -3271,7 +3285,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>42</v>
+        <v>190</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>191</v>
@@ -3281,7 +3295,7 @@
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15" t="s">
-        <v>42</v>
+        <v>200</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>202</v>
@@ -3294,7 +3308,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>179</v>
+        <v>42</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>191</v>
@@ -3304,7 +3318,7 @@
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>202</v>
@@ -3317,7 +3331,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>191</v>
@@ -3336,36 +3350,46 @@
       <c r="I17" s="12"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="11">
+      <c r="A18" s="14">
         <v>17</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="12"/>
+      <c r="B18" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>202</v>
+      </c>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="11">
+      <c r="A19" s="14">
         <v>18</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="12"/>
+      <c r="B19" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>202</v>
+      </c>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
     </row>
@@ -3373,39 +3397,39 @@
       <c r="A20" s="14">
         <v>19</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>202</v>
-      </c>
+      <c r="B20" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="12"/>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="11">
+      <c r="A21" s="14">
         <v>20</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="12"/>
+      <c r="B21" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>202</v>
+      </c>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
     </row>
@@ -3413,22 +3437,16 @@
       <c r="A22" s="14">
         <v>21</v>
       </c>
-      <c r="B22" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>202</v>
-      </c>
+      <c r="B22" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="12"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
     </row>
@@ -3437,7 +3455,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>158</v>
+        <v>54</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>191</v>
@@ -3447,7 +3465,7 @@
       </c>
       <c r="E23" s="15"/>
       <c r="F23" s="15" t="s">
-        <v>158</v>
+        <v>6</v>
       </c>
       <c r="G23" s="15" t="s">
         <v>202</v>
@@ -3460,7 +3478,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>191</v>
@@ -3483,11 +3501,9 @@
         <v>24</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>191</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="C25" s="16"/>
       <c r="D25" s="16" t="s">
         <v>191</v>
       </c>
@@ -3506,7 +3522,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>191</v>
@@ -3525,28 +3541,34 @@
       <c r="I26" s="12"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="11">
+      <c r="A27" s="14">
         <v>26</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12" t="s">
+      <c r="B27" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="G27" s="12"/>
+      <c r="G27" s="15" t="s">
+        <v>202</v>
+      </c>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="11">
+      <c r="A28" s="14">
         <v>27</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -3554,16 +3576,15 @@
       <c r="F28" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G28" s="12"/>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="11">
+      <c r="A29" s="14">
         <v>28</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
@@ -3576,11 +3597,11 @@
       <c r="I29" s="12"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="11">
+      <c r="A30" s="14">
         <v>29</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
@@ -3593,28 +3614,28 @@
       <c r="I30" s="12"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="11">
+      <c r="A31" s="14">
         <v>30</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="11">
+      <c r="A32" s="14">
         <v>31</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
@@ -3627,28 +3648,28 @@
       <c r="I32" s="12"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="11">
+      <c r="A33" s="14">
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
       <c r="I33" s="12"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="11">
+      <c r="A34" s="14">
         <v>33</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
@@ -3661,62 +3682,62 @@
       <c r="I34" s="12"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="11">
+      <c r="A35" s="14">
         <v>34</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="11">
+      <c r="A36" s="14">
         <v>35</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12" t="s">
-        <v>145</v>
+        <v>194</v>
       </c>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="11">
+      <c r="A37" s="14">
         <v>36</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12" t="s">
-        <v>194</v>
+        <v>145</v>
       </c>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
       <c r="I37" s="12"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="11">
+      <c r="A38" s="14">
         <v>37</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
@@ -3729,11 +3750,11 @@
       <c r="I38" s="12"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="11">
+      <c r="A39" s="14">
         <v>38</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
@@ -3745,9 +3766,26 @@
       <c r="H39" s="12"/>
       <c r="I39" s="12"/>
     </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="14">
+        <v>39</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F39">
-    <sortCondition ref="F1:F39"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F40">
+    <sortCondition ref="F1:F40"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
CAP NHAT NGÀY 11 THANG 09 NAM 2023
</commit_message>
<xml_diff>
--- a/Luận văn GITHUB.xlsx
+++ b/Luận văn GITHUB.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LVTN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC292D5-710D-4B27-8D55-868E6CBF46B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C109C6FA-D07D-4CAF-94EE-E799E0B24769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{F613D93C-81B0-455C-B6DD-EA6E57B6EA76}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="204">
   <si>
     <t>STT</t>
   </si>
@@ -635,10 +635,10 @@
     <t>Trạng thái cài đặt</t>
   </si>
   <si>
-    <t>Đã cài đặt, chưa kiểm tra</t>
-  </si>
-  <si>
     <t>Hình Minh Họa</t>
+  </si>
+  <si>
+    <t>Tình trạng kiểm tra</t>
   </si>
 </sst>
 </file>
@@ -731,7 +731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -760,18 +760,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1093,6 +1082,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F61E465-1856-435F-BB9A-67E68A09B550}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -1891,6 +1881,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24DBD2CB-C7AF-473B-883D-FF096ADFC834}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
@@ -2945,10 +2936,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76849178-7D8E-40D5-805E-F1C496D5B8E9}">
-  <dimension ref="A1:I45"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2959,12 +2951,13 @@
     <col min="4" max="4" width="17.77734375" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2983,853 +2976,1029 @@
       <c r="F1" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="14">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15" t="s">
+      <c r="C2" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H2" s="11">
+      <c r="G2" s="11">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13" t="str">
+        <f>IF(G2 = 0, "Chưa cài đặt", IF(G2 = 1," Đã cài đặt chưa kiểm tra",IF(G2 = 2,"Đã kiểm tra","Lỗi")))</f>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I2" s="11">
         <f>COUNTIF(D2:D40,"x")</f>
-        <v>23</v>
-      </c>
-      <c r="I2" s="11">
+        <v>36</v>
+      </c>
+      <c r="J2" s="11">
         <f>COUNTIF(E2:E40,"x")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="14">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15" t="s">
+      <c r="C3" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="11">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13" t="str">
+        <f t="shared" ref="H3:H39" si="0">IF(G3 = 0, "Chưa cài đặt", IF(G3 = 1," Đã cài đặt chưa kiểm tra",IF(G3 = 2,"Đã kiểm tra","Lỗi")))</f>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="G4" s="11">
+        <v>1</v>
+      </c>
+      <c r="H4" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="G5" s="11">
+        <v>1</v>
+      </c>
+      <c r="H5" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="G6" s="11">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="G7" s="11">
+        <v>1</v>
+      </c>
+      <c r="H7" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G8" s="11">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G9" s="11">
+        <v>1</v>
+      </c>
+      <c r="H9" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="11">
+        <v>1</v>
+      </c>
+      <c r="H10" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="11">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="G12" s="11">
+        <v>1</v>
+      </c>
+      <c r="H12" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="G13" s="11">
+        <v>1</v>
+      </c>
+      <c r="H13" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="11">
+        <v>13</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="14">
-        <v>3</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15" t="s">
-        <v>195</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="14">
-        <v>4</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
-        <v>5</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="14">
-        <v>6</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="14">
-        <v>7</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="14">
-        <v>8</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="14">
-        <v>9</v>
-      </c>
-      <c r="B10" s="15" t="s">
+      <c r="C14" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="G14" s="11">
+        <v>1</v>
+      </c>
+      <c r="H14" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="11">
+        <v>14</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="G15" s="11">
+        <v>1</v>
+      </c>
+      <c r="H15" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="11">
+        <v>15</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="11">
+        <v>1</v>
+      </c>
+      <c r="H16" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="11">
+        <v>16</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="11">
+        <v>1</v>
+      </c>
+      <c r="H17" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="11">
+        <v>17</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="11">
+        <v>1</v>
+      </c>
+      <c r="H18" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="11">
+        <v>18</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="11">
+        <v>1</v>
+      </c>
+      <c r="H19" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="11">
+        <v>19</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="11">
+        <v>1</v>
+      </c>
+      <c r="H20" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="11">
+        <v>20</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="11">
+        <v>1</v>
+      </c>
+      <c r="H21" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="11">
+        <v>21</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="11">
+        <v>1</v>
+      </c>
+      <c r="H22" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="11">
+        <v>22</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="11">
+        <v>1</v>
+      </c>
+      <c r="H23" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="11">
+        <v>23</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="G24" s="11">
+        <v>1</v>
+      </c>
+      <c r="H24" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="11">
         <v>24</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="14">
-        <v>10</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="14">
-        <v>11</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="14">
-        <v>12</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="14">
-        <v>14</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="14">
-        <v>15</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="14">
-        <v>16</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="14">
-        <v>17</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="14">
-        <v>18</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="14">
-        <v>19</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="14">
-        <v>20</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="14">
-        <v>21</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="14">
-        <v>22</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="14">
-        <v>23</v>
-      </c>
-      <c r="B24" s="15" t="s">
+      <c r="B25" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="C24" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15" t="s">
+      <c r="G25" s="11">
+        <v>1</v>
+      </c>
+      <c r="H25" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="11">
+        <v>25</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G24" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="14">
-        <v>24</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15" t="s">
+      <c r="G26" s="11">
+        <v>1</v>
+      </c>
+      <c r="H26" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="11">
+        <v>26</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G25" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="14">
-        <v>25</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15" t="s">
+      <c r="G27" s="11">
+        <v>1</v>
+      </c>
+      <c r="H27" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="11">
+        <v>27</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G26" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="14">
-        <v>26</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15" t="s">
+      <c r="G28" s="11">
+        <v>1</v>
+      </c>
+      <c r="H28" s="13" t="str">
+        <f>IF(G28 = 0, "Chưa cài đặt", IF(G28 = 1," Đã cài đặt chưa kiểm tra",IF(G28 = 2,"Đã kiểm tra","Lỗi")))</f>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="11">
+        <v>28</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G27" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="14">
-        <v>27</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15" t="s">
+      <c r="G29" s="11">
+        <v>1</v>
+      </c>
+      <c r="H29" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="11">
+        <v>29</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="14">
-        <v>28</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15" t="s">
+      <c r="G30" s="11">
+        <v>1</v>
+      </c>
+      <c r="H30" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="11">
+        <v>30</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="14">
-        <v>29</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="14">
-        <v>30</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
+      <c r="G31" s="11">
+        <v>1</v>
+      </c>
+      <c r="H31" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
       <c r="I31" s="12"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="14">
+      <c r="J31" s="12"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="11">
         <v>31</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15" t="s">
+      <c r="C32" s="14"/>
+      <c r="D32" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
+      <c r="G32" s="11">
+        <v>1</v>
+      </c>
+      <c r="H32" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
       <c r="I32" s="12"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="14">
+      <c r="J32" s="12"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="11">
         <v>32</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15" t="s">
+      <c r="C33" s="14"/>
+      <c r="D33" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
+      <c r="G33" s="11">
+        <v>1</v>
+      </c>
+      <c r="H33" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
       <c r="I33" s="12"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="14">
+      <c r="J33" s="12"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="11">
         <v>33</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15" t="s">
+      <c r="C34" s="14"/>
+      <c r="D34" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
+      <c r="G34" s="11">
+        <v>1</v>
+      </c>
+      <c r="H34" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
       <c r="I34" s="12"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="14">
+      <c r="J34" s="12"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="11">
         <v>34</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15" t="s">
+      <c r="C35" s="14"/>
+      <c r="D35" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
+      <c r="G35" s="11">
+        <v>1</v>
+      </c>
+      <c r="H35" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
       <c r="I35" s="12"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="14">
+      <c r="J35" s="12"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="11">
         <v>35</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15" t="s">
+      <c r="C36" s="14"/>
+      <c r="D36" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
+      <c r="G36" s="11">
+        <v>1</v>
+      </c>
+      <c r="H36" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
       <c r="I36" s="12"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="14">
+      <c r="J36" s="12"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="11">
         <v>36</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="G37" s="11">
+        <v>1</v>
+      </c>
+      <c r="H37" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
+      </c>
       <c r="I37" s="12"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="14">
+      <c r="J37" s="12"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="11">
         <v>37</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15" t="s">
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
+      <c r="G38" s="11">
+        <v>0</v>
+      </c>
+      <c r="H38" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>Chưa cài đặt</v>
+      </c>
       <c r="I38" s="12"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="14">
+      <c r="J38" s="12"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="11">
         <v>38</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15" t="s">
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
+      <c r="G39" s="11">
+        <v>0</v>
+      </c>
+      <c r="H39" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>Chưa cài đặt</v>
+      </c>
       <c r="I39" s="12"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="14">
+      <c r="J39" s="12"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="11">
         <v>39</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15" t="s">
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
+      <c r="G40" s="11">
+        <v>0</v>
+      </c>
+      <c r="H40" s="13" t="str">
+        <f>IF(G40 = 0, "Chưa cài đặt", IF(G40 = 1," Đã cài đặt chưa kiểm tra",IF(G40 = 2,"Đã kiểm tra","Lỗi")))</f>
+        <v>Chưa cài đặt</v>
+      </c>
       <c r="I40" s="12"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="17"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="17"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="17"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="17"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="17"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
+      <c r="J40" s="12"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F40">

</xml_diff>

<commit_message>
cap nhat nhay 16/10/2023
</commit_message>
<xml_diff>
--- a/Luận văn GITHUB.xlsx
+++ b/Luận văn GITHUB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LVTN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C109C6FA-D07D-4CAF-94EE-E799E0B24769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14707ADB-D49B-40A6-AB97-FE6CCE7DAA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{F613D93C-81B0-455C-B6DD-EA6E57B6EA76}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="204">
   <si>
     <t>STT</t>
   </si>
@@ -690,7 +690,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -700,6 +700,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF66"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -759,10 +765,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1884,8 +1890,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F8:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2937,1072 +2943,1197 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76849178-7D8E-40D5-805E-F1C496D5B8E9}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.77734375" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12" t="s">
+      <c r="C2" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="G2" s="11">
-        <v>1</v>
-      </c>
-      <c r="H2" s="13" t="str">
-        <f>IF(G2 = 0, "Chưa cài đặt", IF(G2 = 1," Đã cài đặt chưa kiểm tra",IF(G2 = 2,"Đã kiểm tra","Lỗi")))</f>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I2" s="11">
-        <f>COUNTIF(D2:D40,"x")</f>
-        <v>36</v>
+      <c r="H2" s="11">
+        <v>2</v>
+      </c>
+      <c r="I2" s="14" t="str">
+        <f>IF(H2 = 0, "Chưa cài đặt", IF(H2 = 1," Đã cài đặt chưa kiểm tra",IF(H2 = 2,"Đã kiểm tra","Lỗi")))</f>
+        <v>Đã kiểm tra</v>
       </c>
       <c r="J2" s="11">
         <f>COUNTIF(E2:E40,"x")</f>
+        <v>39</v>
+      </c>
+      <c r="K2" s="11">
+        <f>COUNTIF(F2:F40,"x")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12" t="s">
+      <c r="C3" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="G3" s="11">
-        <v>1</v>
-      </c>
-      <c r="H3" s="13" t="str">
-        <f t="shared" ref="H3:H39" si="0">IF(G3 = 0, "Chưa cài đặt", IF(G3 = 1," Đã cài đặt chưa kiểm tra",IF(G3 = 2,"Đã kiểm tra","Lỗi")))</f>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I3" s="12"/>
+      <c r="H3" s="11">
+        <v>2</v>
+      </c>
+      <c r="I3" s="14" t="str">
+        <f t="shared" ref="I3:I39" si="0">IF(H3 = 0, "Chưa cài đặt", IF(H3 = 1," Đã cài đặt chưa kiểm tra",IF(H3 = 2,"Đã kiểm tra","Lỗi")))</f>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J3" s="12"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3" s="12"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12" t="s">
+      <c r="C4" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="G4" s="11">
-        <v>1</v>
-      </c>
-      <c r="H4" s="13" t="str">
+      <c r="H4" s="11">
+        <v>2</v>
+      </c>
+      <c r="I4" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I4" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J4" s="12"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4" s="12"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12" t="s">
+      <c r="C5" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="G5" s="11">
-        <v>1</v>
-      </c>
-      <c r="H5" s="13" t="str">
+      <c r="H5" s="11">
+        <v>2</v>
+      </c>
+      <c r="I5" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I5" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5" s="12"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12" t="s">
+      <c r="C6" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="G6" s="11">
-        <v>1</v>
-      </c>
-      <c r="H6" s="13" t="str">
+      <c r="H6" s="11">
+        <v>2</v>
+      </c>
+      <c r="I6" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I6" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J6" s="12"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6" s="12"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12" t="s">
+      <c r="C7" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="G7" s="11">
-        <v>1</v>
-      </c>
-      <c r="H7" s="13" t="str">
+      <c r="H7" s="11">
+        <v>2</v>
+      </c>
+      <c r="I7" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I7" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J7" s="12"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7" s="12"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12" t="s">
+      <c r="C8" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="G8" s="11">
-        <v>1</v>
-      </c>
-      <c r="H8" s="13" t="str">
+      <c r="H8" s="11">
+        <v>2</v>
+      </c>
+      <c r="I8" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I8" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J8" s="12"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8" s="12"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12" t="s">
+      <c r="C9" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="G9" s="11">
-        <v>1</v>
-      </c>
-      <c r="H9" s="13" t="str">
+      <c r="H9" s="11">
+        <v>2</v>
+      </c>
+      <c r="I9" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I9" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J9" s="12"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9" s="12"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="12" t="s">
+      <c r="C10" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="11">
-        <v>1</v>
-      </c>
-      <c r="H10" s="13" t="str">
+      <c r="H10" s="11">
+        <v>2</v>
+      </c>
+      <c r="I10" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I10" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J10" s="12"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10" s="12"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12" t="s">
+      <c r="C11" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="11">
-        <v>1</v>
-      </c>
-      <c r="H11" s="13" t="str">
+      <c r="H11" s="11">
+        <v>2</v>
+      </c>
+      <c r="I11" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I11" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J11" s="12"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K11" s="12"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12" t="s">
+      <c r="C12" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="G12" s="11">
-        <v>1</v>
-      </c>
-      <c r="H12" s="13" t="str">
+      <c r="H12" s="11">
+        <v>2</v>
+      </c>
+      <c r="I12" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I12" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J12" s="12"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K12" s="12"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>12</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12" t="s">
+      <c r="C13" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="G13" s="11">
-        <v>1</v>
-      </c>
-      <c r="H13" s="13" t="str">
+      <c r="H13" s="11">
+        <v>2</v>
+      </c>
+      <c r="I13" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I13" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J13" s="12"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K13" s="12"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12" t="s">
+      <c r="C14" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="G14" s="11">
-        <v>1</v>
-      </c>
-      <c r="H14" s="13" t="str">
+      <c r="H14" s="11">
+        <v>2</v>
+      </c>
+      <c r="I14" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I14" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J14" s="12"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K14" s="12"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12" t="s">
+      <c r="C15" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="G15" s="11">
-        <v>1</v>
-      </c>
-      <c r="H15" s="13" t="str">
+      <c r="H15" s="11">
+        <v>2</v>
+      </c>
+      <c r="I15" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I15" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J15" s="12"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K15" s="12"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
         <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12" t="s">
+      <c r="C16" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="11">
-        <v>1</v>
-      </c>
-      <c r="H16" s="13" t="str">
+      <c r="H16" s="11">
+        <v>2</v>
+      </c>
+      <c r="I16" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I16" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>16</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="11">
-        <v>1</v>
-      </c>
-      <c r="H17" s="13" t="str">
+      <c r="C17" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="11">
+        <v>2</v>
+      </c>
+      <c r="I17" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I17" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J17" s="12"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="11">
-        <v>1</v>
-      </c>
-      <c r="H18" s="13" t="str">
+      <c r="C18" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="11">
+        <v>2</v>
+      </c>
+      <c r="I18" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I18" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J18" s="12"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18" s="12"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="11">
         <v>18</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="11">
-        <v>1</v>
-      </c>
-      <c r="H19" s="13" t="str">
+      <c r="C19" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="11">
+        <v>2</v>
+      </c>
+      <c r="I19" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I19" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J19" s="12"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19" s="12"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="11">
         <v>19</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" s="11">
-        <v>1</v>
-      </c>
-      <c r="H20" s="13" t="str">
+      <c r="C20" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="11">
+        <v>2</v>
+      </c>
+      <c r="I20" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I20" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J20" s="12"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
         <v>20</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="11">
-        <v>1</v>
-      </c>
-      <c r="H21" s="13" t="str">
+      <c r="C21" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="11">
+        <v>2</v>
+      </c>
+      <c r="I21" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I21" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J21" s="12"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21" s="12"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="11">
         <v>21</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" s="11">
-        <v>1</v>
-      </c>
-      <c r="H22" s="13" t="str">
+      <c r="C22" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="11">
+        <v>2</v>
+      </c>
+      <c r="I22" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I22" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J22" s="12"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22" s="12"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="11">
         <v>22</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G23" s="11">
-        <v>1</v>
-      </c>
-      <c r="H23" s="13" t="str">
+      <c r="C23" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="11">
+        <v>2</v>
+      </c>
+      <c r="I23" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I23" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J23" s="12"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K23" s="12"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="11">
         <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="C24" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12" t="s">
+      <c r="C24" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G24" s="11">
-        <v>1</v>
-      </c>
-      <c r="H24" s="13" t="str">
+      <c r="H24" s="11">
+        <v>2</v>
+      </c>
+      <c r="I24" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I24" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J24" s="12"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
         <v>24</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12" t="s">
+      <c r="C25" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G25" s="11">
-        <v>1</v>
-      </c>
-      <c r="H25" s="13" t="str">
+      <c r="H25" s="11">
+        <v>2</v>
+      </c>
+      <c r="I25" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I25" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J25" s="12"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K25" s="12"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="11">
         <v>25</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12" t="s">
+      <c r="C26" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G26" s="11">
-        <v>1</v>
-      </c>
-      <c r="H26" s="13" t="str">
+      <c r="H26" s="11">
+        <v>2</v>
+      </c>
+      <c r="I26" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I26" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J26" s="12"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K26" s="12"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <v>26</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="C27" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12" t="s">
+      <c r="C27" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G27" s="11">
-        <v>1</v>
-      </c>
-      <c r="H27" s="13" t="str">
+      <c r="H27" s="11">
+        <v>2</v>
+      </c>
+      <c r="I27" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I27" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J27" s="12"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K27" s="12"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="11">
         <v>27</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12" t="s">
+      <c r="C28" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G28" s="11">
-        <v>1</v>
-      </c>
-      <c r="H28" s="13" t="str">
-        <f>IF(G28 = 0, "Chưa cài đặt", IF(G28 = 1," Đã cài đặt chưa kiểm tra",IF(G28 = 2,"Đã kiểm tra","Lỗi")))</f>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I28" s="12"/>
+      <c r="H28" s="11">
+        <v>2</v>
+      </c>
+      <c r="I28" s="14" t="str">
+        <f>IF(H28 = 0, "Chưa cài đặt", IF(H28 = 1," Đã cài đặt chưa kiểm tra",IF(H28 = 2,"Đã kiểm tra","Lỗi")))</f>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J28" s="12"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K28" s="12"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="11">
         <v>28</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12" t="s">
+      <c r="C29" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G29" s="11">
-        <v>1</v>
-      </c>
-      <c r="H29" s="13" t="str">
+      <c r="H29" s="11">
+        <v>2</v>
+      </c>
+      <c r="I29" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I29" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J29" s="12"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K29" s="12"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <v>29</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12" t="s">
+      <c r="C30" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G30" s="11">
-        <v>1</v>
-      </c>
-      <c r="H30" s="13" t="str">
+      <c r="H30" s="11">
+        <v>2</v>
+      </c>
+      <c r="I30" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I30" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J30" s="12"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K30" s="12"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
         <v>30</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12" t="s">
+      <c r="C31" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G31" s="11">
-        <v>1</v>
-      </c>
-      <c r="H31" s="13" t="str">
+      <c r="H31" s="11">
+        <v>2</v>
+      </c>
+      <c r="I31" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I31" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J31" s="12"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K31" s="12"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="11">
         <v>31</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12" t="s">
+      <c r="C32" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="G32" s="11">
-        <v>1</v>
-      </c>
-      <c r="H32" s="13" t="str">
+      <c r="H32" s="11">
+        <v>2</v>
+      </c>
+      <c r="I32" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I32" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J32" s="12"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K32" s="12"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="11">
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12" t="s">
+      <c r="C33" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="G33" s="11">
-        <v>1</v>
-      </c>
-      <c r="H33" s="13" t="str">
+      <c r="H33" s="11">
+        <v>2</v>
+      </c>
+      <c r="I33" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I33" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J33" s="12"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K33" s="12"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="11">
         <v>33</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12" t="s">
+      <c r="C34" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="G34" s="11">
-        <v>1</v>
-      </c>
-      <c r="H34" s="13" t="str">
+      <c r="H34" s="11">
+        <v>2</v>
+      </c>
+      <c r="I34" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I34" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J34" s="12"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K34" s="12"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="11">
         <v>34</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12" t="s">
+      <c r="C35" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="G35" s="11">
-        <v>1</v>
-      </c>
-      <c r="H35" s="13" t="str">
+      <c r="H35" s="11">
+        <v>2</v>
+      </c>
+      <c r="I35" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I35" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J35" s="12"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K35" s="12"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="11">
         <v>35</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12" t="s">
+      <c r="C36" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="G36" s="11">
-        <v>1</v>
-      </c>
-      <c r="H36" s="13" t="str">
+      <c r="H36" s="11">
+        <v>2</v>
+      </c>
+      <c r="I36" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I36" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J36" s="12"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K36" s="12"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="11">
         <v>36</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12" t="s">
+      <c r="C37" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D37" s="13"/>
+      <c r="E37" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="G37" s="11">
-        <v>1</v>
-      </c>
-      <c r="H37" s="13" t="str">
+      <c r="H37" s="11">
+        <v>2</v>
+      </c>
+      <c r="I37" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> Đã cài đặt chưa kiểm tra</v>
-      </c>
-      <c r="I37" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J37" s="12"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K37" s="12"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="11">
         <v>37</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12" t="s">
+      <c r="C38" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="G38" s="11">
-        <v>0</v>
-      </c>
-      <c r="H38" s="13" t="str">
+      <c r="H38" s="11">
+        <v>2</v>
+      </c>
+      <c r="I38" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>Chưa cài đặt</v>
-      </c>
-      <c r="I38" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J38" s="12"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K38" s="12"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="11">
         <v>38</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12" t="s">
+      <c r="C39" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="G39" s="11">
-        <v>0</v>
-      </c>
-      <c r="H39" s="13" t="str">
+      <c r="H39" s="11">
+        <v>2</v>
+      </c>
+      <c r="I39" s="14" t="str">
         <f t="shared" si="0"/>
-        <v>Chưa cài đặt</v>
-      </c>
-      <c r="I39" s="12"/>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J39" s="12"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K39" s="12"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="11">
         <v>39</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12" t="s">
+      <c r="C40" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="G40" s="11">
-        <v>0</v>
-      </c>
-      <c r="H40" s="13" t="str">
-        <f>IF(G40 = 0, "Chưa cài đặt", IF(G40 = 1," Đã cài đặt chưa kiểm tra",IF(G40 = 2,"Đã kiểm tra","Lỗi")))</f>
-        <v>Chưa cài đặt</v>
-      </c>
-      <c r="I40" s="12"/>
+      <c r="H40" s="11">
+        <v>2</v>
+      </c>
+      <c r="I40" s="14" t="str">
+        <f>IF(H40 = 0, "Chưa cài đặt", IF(H40 = 1," Đã cài đặt chưa kiểm tra",IF(H40 = 2,"Đã kiểm tra","Lỗi")))</f>
+        <v>Đã kiểm tra</v>
+      </c>
       <c r="J40" s="12"/>
+      <c r="K40" s="12"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F40">
-    <sortCondition ref="F1:F40"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G40">
+    <sortCondition ref="G1:G40"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>